<commit_message>
Could fix the issue when getting a resource after a post
</commit_message>
<xml_diff>
--- a/src/main/resources/dataFiles/CustomerData.xlsx
+++ b/src/main/resources/dataFiles/CustomerData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/dataFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/src/main/resources/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8DADA8-EBB6-DE44-9199-0E775727B5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5981960B-506D-C940-9A7C-3479C716C51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="3" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A654EF-E738-EF45-9F68-AF93F1F7392E}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +617,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE76BCDD-0C74-9841-AE96-F9136D912BF6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Improved putCustomerBillingAddress by adding a custom comparator
</commit_message>
<xml_diff>
--- a/src/main/resources/dataFiles/CustomerData.xlsx
+++ b/src/main/resources/dataFiles/CustomerData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/src/main/resources/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5981960B-506D-C940-9A7C-3479C716C51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6716EEBD-9602-A74A-A9CA-36390B331542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>email</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>v-neck-t-shirt</t>
+  </si>
+  <si>
+    <t>Anila</t>
+  </si>
+  <si>
+    <t>Niles</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,10 +626,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added more validations to some product tests
</commit_message>
<xml_diff>
--- a/src/main/resources/dataFiles/CustomerData.xlsx
+++ b/src/main/resources/dataFiles/CustomerData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelrodriguez/repo/apiTesting_challenge/src/main/resources/dataFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel.rodriguez/repo/apiTesting_challenge/src/main/resources/dataFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6716EEBD-9602-A74A-A9CA-36390B331542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D600526-980C-6342-83D1-6A7E716C65A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41280" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="1" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
+    <workbookView xWindow="39340" yWindow="760" windowWidth="32660" windowHeight="20540" activeTab="3" xr2:uid="{141FC98E-6DB1-9A46-8C80-630429BF8D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A654EF-E738-EF45-9F68-AF93F1F7392E}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE76BCDD-0C74-9841-AE96-F9136D912BF6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>